<commit_message>
Fixed the chrome parallel execution issue.
</commit_message>
<xml_diff>
--- a/POM_DataDriven/Excels/Testdata.xlsx
+++ b/POM_DataDriven/Excels/Testdata.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8820" tabRatio="779"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8820" tabRatio="779" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="login" sheetId="2" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="40">
   <si>
     <t>TC ID</t>
   </si>
@@ -133,9 +133,6 @@
   </si>
   <si>
     <t>ParentAccount</t>
-  </si>
-  <si>
-    <t>Account Record</t>
   </si>
   <si>
     <t>Edge Communication</t>
@@ -527,7 +524,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
@@ -596,13 +593,13 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D5" t="s">
         <v>7</v>
@@ -767,7 +764,7 @@
         <v>30</v>
       </c>
       <c r="D2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -777,21 +774,20 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -804,11 +800,8 @@
       <c r="D1" t="s">
         <v>31</v>
       </c>
-      <c r="E1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>34</v>
       </c>
@@ -819,9 +812,6 @@
         <v>29</v>
       </c>
       <c r="D2" t="s">
-        <v>29</v>
-      </c>
-      <c r="E2" t="s">
         <v>29</v>
       </c>
     </row>

</xml_diff>